<commit_message>
Doc and other stuff
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journaux_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Finalisation de la page d'achat sur le Wireframe.</t>
   </si>
   <si>
-    <t>Developpement</t>
-  </si>
-  <si>
     <t>Rogner automatiquement les images du carousel.</t>
   </si>
   <si>
@@ -150,6 +147,21 @@
   </si>
   <si>
     <t>Finalisation de la documentation avec Romain.</t>
+  </si>
+  <si>
+    <t>Révision du cours ICT-151 car nous avons fini le projet.</t>
+  </si>
+  <si>
+    <t>Révision</t>
+  </si>
+  <si>
+    <t>Prise de note pour les feuilles d'aide d'examen.</t>
+  </si>
+  <si>
+    <t>Mise des commentaires sur le code avec Romain.</t>
+  </si>
+  <si>
+    <t>Analyse de sprint et autres dans la documentation</t>
   </si>
 </sst>
 </file>
@@ -655,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1099"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,10 +1129,10 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="6"/>
@@ -1168,7 +1180,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" s="15"/>
     </row>
@@ -1187,13 +1199,13 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="15" t="s">
         <v>25</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1211,10 +1223,10 @@
         <v>1.736111111111116E-2</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="G24" s="15"/>
     </row>
@@ -1233,13 +1245,13 @@
         <v>5.6250000000000022E-2</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1257,13 +1269,13 @@
         <v>2.5694444444444464E-2</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1284,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="15"/>
     </row>
@@ -1303,10 +1315,10 @@
         <v>3.2638888888888773E-2</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G28" s="18"/>
     </row>
@@ -1328,7 +1340,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G29" s="15"/>
     </row>
@@ -1350,10 +1362,10 @@
         <v>7</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1374,10 +1386,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1395,13 +1407,13 @@
         <v>1.4583333333333393E-2</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1419,13 +1431,13 @@
         <v>6.597222222222221E-2</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1435,79 +1447,133 @@
       <c r="B34" s="8">
         <v>0.5625</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="8">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D34" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>-0.5625</v>
+        <v>0.14236111111111116</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>45013</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D35" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>2.8472222222222232E-2</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G35" s="15"/>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>45014</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="D36" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>45014</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D37" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>45014</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D38" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>5.8333333333333348E-2</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="15"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+      <c r="F38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>45015</v>
+      </c>
+      <c r="B39" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D39" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="G39" s="17"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>